<commit_message>
Forgot to save a file
</commit_message>
<xml_diff>
--- a/scraper_and_data/Plants-Species-Origins.xlsx
+++ b/scraper_and_data/Plants-Species-Origins.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ameliamlu12\Documents\Fall 2015\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26423"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10060"/>
+    <workbookView xWindow="0" yWindow="3440" windowWidth="19200" windowHeight="15000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,9 +12,11 @@
   <definedNames>
     <definedName name="Regions">Sheet1!$L$2:$L$10</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="191">
   <si>
     <t>Species</t>
   </si>
@@ -598,13 +595,16 @@
   </si>
   <si>
     <t>NOTE: Can figure out if we really need it</t>
+  </si>
+  <si>
+    <t>Astragalus nakaianus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,8 +626,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -664,6 +680,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF800080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -674,10 +696,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -693,8 +717,11 @@
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -758,7 +785,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -793,7 +820,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -970,7 +997,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -978,19 +1005,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L102"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="28.81640625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="46.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1004,7 +1031,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1018,7 +1045,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1032,7 +1059,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1046,7 +1073,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1060,7 +1087,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12">
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
@@ -1074,7 +1101,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -1088,7 +1115,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1102,7 +1129,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12">
       <c r="A9" s="4" t="s">
         <v>17</v>
       </c>
@@ -1113,7 +1140,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1127,7 +1154,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12">
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
@@ -1135,7 +1162,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1146,7 +1173,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1157,7 +1184,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1168,7 +1195,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -1179,7 +1206,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1190,7 +1217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1201,7 +1228,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3">
       <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
@@ -1209,7 +1236,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1220,7 +1247,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1231,7 +1258,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1242,7 +1269,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
         <v>42</v>
       </c>
@@ -1253,7 +1280,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
         <v>44</v>
       </c>
@@ -1264,7 +1291,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3">
       <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
@@ -1272,7 +1299,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3">
       <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
@@ -1280,7 +1307,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3">
       <c r="A26" s="5" t="s">
         <v>50</v>
       </c>
@@ -1291,7 +1318,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1302,7 +1329,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3">
       <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
@@ -1310,7 +1337,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3">
       <c r="A29" s="4" t="s">
         <v>56</v>
       </c>
@@ -1318,7 +1345,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3">
       <c r="A30" t="s">
         <v>57</v>
       </c>
@@ -1329,7 +1356,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3">
       <c r="A31" s="5" t="s">
         <v>58</v>
       </c>
@@ -1340,7 +1367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3">
       <c r="A32" t="s">
         <v>60</v>
       </c>
@@ -1351,7 +1378,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3">
       <c r="A33" s="5" t="s">
         <v>62</v>
       </c>
@@ -1362,7 +1389,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3">
       <c r="A34" s="3" t="s">
         <v>64</v>
       </c>
@@ -1373,7 +1400,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -1384,7 +1411,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3">
       <c r="A36" s="6" t="s">
         <v>68</v>
       </c>
@@ -1392,7 +1419,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1403,7 +1430,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3">
       <c r="A38" t="s">
         <v>71</v>
       </c>
@@ -1414,7 +1441,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3">
       <c r="A39" t="s">
         <v>72</v>
       </c>
@@ -1425,7 +1452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3">
       <c r="A40" s="5" t="s">
         <v>73</v>
       </c>
@@ -1436,7 +1463,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3">
       <c r="A41" s="3" t="s">
         <v>75</v>
       </c>
@@ -1444,7 +1471,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
         <v>77</v>
       </c>
@@ -1452,7 +1479,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -1463,7 +1490,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3">
       <c r="A44" s="4" t="s">
         <v>81</v>
       </c>
@@ -1471,7 +1498,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3">
       <c r="A45" s="4" t="s">
         <v>83</v>
       </c>
@@ -1479,7 +1506,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3">
       <c r="A46" t="s">
         <v>85</v>
       </c>
@@ -1490,7 +1517,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3">
       <c r="A47" s="4" t="s">
         <v>87</v>
       </c>
@@ -1498,7 +1525,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3">
       <c r="A48" t="s">
         <v>89</v>
       </c>
@@ -1509,7 +1536,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3">
       <c r="A49" s="6" t="s">
         <v>90</v>
       </c>
@@ -1517,7 +1544,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3">
       <c r="A50" s="4" t="s">
         <v>91</v>
       </c>
@@ -1525,7 +1552,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3">
       <c r="A51" t="s">
         <v>93</v>
       </c>
@@ -1536,7 +1563,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3">
       <c r="A52" s="7" t="s">
         <v>95</v>
       </c>
@@ -1547,7 +1574,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -1558,7 +1585,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3">
       <c r="A54" t="s">
         <v>98</v>
       </c>
@@ -1569,7 +1596,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3">
       <c r="A55" t="s">
         <v>100</v>
       </c>
@@ -1580,7 +1607,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3">
       <c r="A56" t="s">
         <v>101</v>
       </c>
@@ -1591,7 +1618,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3">
       <c r="A57" t="s">
         <v>103</v>
       </c>
@@ -1602,7 +1629,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3">
       <c r="A58" t="s">
         <v>104</v>
       </c>
@@ -1613,216 +1640,210 @@
         <v>112</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="4" t="s">
+    <row r="59" spans="1:3">
+      <c r="A59" s="11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B60" s="9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" t="s">
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
         <v>108</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B61" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
         <v>110</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B62" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C61" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
+      <c r="C62" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
         <v>118</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B63" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
+    <row r="64" spans="1:3">
+      <c r="A64" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B64" s="9" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
         <v>122</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B65" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C65" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
         <v>124</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B66" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C65" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
+      <c r="C66" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
         <v>125</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B67" s="9" t="s">
         <v>6</v>
-      </c>
-      <c r="C66" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>127</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="4" t="s">
+    <row r="68" spans="1:3">
+      <c r="A68" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B69" s="9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
         <v>130</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B70" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="4" t="s">
+    <row r="71" spans="1:3">
+      <c r="A71" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B71" s="9" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
         <v>134</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B72" s="9" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="3" t="s">
+    <row r="73" spans="1:3">
+      <c r="A73" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B73" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C72" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="4" t="s">
+      <c r="C73" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="4" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
         <v>139</v>
       </c>
-      <c r="B74" s="9" t="s">
+      <c r="B75" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="C74" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="4" t="s">
+      <c r="C75" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B76" s="9" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="5" t="s">
+    <row r="77" spans="1:3">
+      <c r="A77" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B77" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C76" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
+      <c r="C77" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
         <v>145</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B78" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
         <v>147</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B79" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C78" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
+      <c r="C79" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
         <v>149</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>150</v>
       </c>
       <c r="B80" s="9" t="s">
         <v>8</v>
@@ -1831,9 +1852,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:4">
       <c r="A81" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B81" s="9" t="s">
         <v>8</v>
@@ -1842,234 +1863,245 @@
         <v>112</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82" s="3" t="s">
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
+        <v>151</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B83" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C82" t="s">
-        <v>112</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="C83" t="s">
+        <v>112</v>
+      </c>
+      <c r="D83" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A83" t="s">
+    <row r="84" spans="1:4">
+      <c r="A84" t="s">
         <v>155</v>
       </c>
-      <c r="B83" s="9" t="s">
+      <c r="B84" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C83" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A84" s="3" t="s">
+      <c r="C84" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B85" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C84" t="s">
-        <v>112</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="C85" t="s">
+        <v>112</v>
+      </c>
+      <c r="D85" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="86" spans="1:4">
+      <c r="A86" t="s">
         <v>157</v>
       </c>
-      <c r="B85" s="9" t="s">
+      <c r="B86" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C85" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A86" s="3" t="s">
+      <c r="C86" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B87" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C86" t="s">
-        <v>112</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="C87" t="s">
+        <v>112</v>
+      </c>
+      <c r="D87" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+    <row r="88" spans="1:4">
+      <c r="A88" t="s">
         <v>159</v>
       </c>
-      <c r="B87" s="9" t="s">
+      <c r="B88" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C87" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A88" s="4" t="s">
+      <c r="C88" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B88" s="9" t="s">
+      <c r="B89" s="9" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+    <row r="90" spans="1:4">
+      <c r="A90" t="s">
         <v>162</v>
       </c>
-      <c r="B89" s="9" t="s">
+      <c r="B90" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C89" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+      <c r="C90" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
         <v>163</v>
       </c>
-      <c r="B90" s="9" t="s">
+      <c r="B91" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C90" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+      <c r="C91" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" t="s">
         <v>164</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="B92" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C91" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A92" s="5" t="s">
+      <c r="C92" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="B92" s="9" t="s">
+      <c r="B93" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A93" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B93" s="9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:4">
       <c r="A94" s="4" t="s">
         <v>168</v>
       </c>
       <c r="B94" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="B95" s="9" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A95" s="4" t="s">
+    <row r="96" spans="1:4">
+      <c r="A96" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B95" s="9" t="s">
+      <c r="B96" s="9" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A96" s="3" t="s">
+    <row r="97" spans="1:4">
+      <c r="A97" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B97" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="C96" t="s">
+      <c r="C97" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A97" s="3" t="s">
+    <row r="98" spans="1:4">
+      <c r="A98" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B97" s="9" t="s">
+      <c r="B98" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D98" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A98" t="s">
+    <row r="99" spans="1:4">
+      <c r="A99" t="s">
         <v>178</v>
       </c>
-      <c r="B98" s="9" t="s">
+      <c r="B99" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C99" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A99" t="s">
+    <row r="100" spans="1:4">
+      <c r="A100" t="s">
         <v>180</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B100" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="C99" t="s">
+      <c r="C100" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A100" s="3" t="s">
+    <row r="101" spans="1:4">
+      <c r="A101" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="B101" s="9" t="s">
         <v>183</v>
-      </c>
-      <c r="C100" t="s">
-        <v>115</v>
-      </c>
-      <c r="D100" s="10" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A101" t="s">
-        <v>185</v>
-      </c>
-      <c r="B101" s="9" t="s">
-        <v>186</v>
       </c>
       <c r="C101" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A102" s="4" t="s">
+      <c r="D101" s="10" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" t="s">
+        <v>185</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C102" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B102" s="9" t="s">
+      <c r="B103" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="D102" s="10" t="s">
+      <c r="D103" s="10" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2080,6 +2112,11 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>